<commit_message>
updating README.md file and Adding Human validation OK
</commit_message>
<xml_diff>
--- a/Developer_Aligned_Validation/DevA_annotations_clean_exact.xlsx
+++ b/Developer_Aligned_Validation/DevA_annotations_clean_exact.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wendkuuni.ouedraogo/Documents/SHORT-PAPERS/CTSES/FOR-GITHUB-REPLCIATION-PACKAGE/CTSES/Developer_Aligned_Validation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4809F8B7-B465-8742-8D3C-1EB7BA0D4545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="34560" yWindow="620" windowWidth="51200" windowHeight="28180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -256,8 +262,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,10 +315,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -320,13 +329,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -364,7 +381,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -398,6 +415,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -432,9 +450,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -607,14 +626,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W9" sqref="W9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="16" max="16" width="6.33203125" customWidth="1"/>
+    <col min="17" max="17" width="47" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -666,783 +694,805 @@
       <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="R1" s="2"/>
     </row>
-    <row r="2" spans="1:17">
-      <c r="A2" t="s">
+    <row r="2" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I2">
-        <v>0.6116</v>
-      </c>
-      <c r="J2">
-        <v>0.7543</v>
-      </c>
-      <c r="K2">
-        <v>0.7202</v>
-      </c>
-      <c r="L2">
+      <c r="I2" s="2">
+        <v>0.61160000000000003</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.75429999999999997</v>
+      </c>
+      <c r="K2" s="2">
+        <v>0.72019999999999995</v>
+      </c>
+      <c r="L2" s="2">
         <v>0.74</v>
       </c>
-      <c r="M2">
-        <v>0.8409</v>
-      </c>
-      <c r="N2">
-        <v>0.8104</v>
-      </c>
-      <c r="O2" t="s">
-        <v>75</v>
-      </c>
-      <c r="P2" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="M2" s="2">
+        <v>0.84089999999999998</v>
+      </c>
+      <c r="N2" s="2">
+        <v>0.81040000000000001</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="R2" s="2"/>
     </row>
-    <row r="3" spans="1:17">
-      <c r="A3" t="s">
+    <row r="3" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I3">
-        <v>0.5659</v>
-      </c>
-      <c r="J3">
-        <v>0.6995</v>
-      </c>
-      <c r="K3">
-        <v>0.6667</v>
-      </c>
-      <c r="L3">
-        <v>0.6861</v>
-      </c>
-      <c r="M3">
-        <v>0.7721</v>
-      </c>
-      <c r="N3">
-        <v>0.7605</v>
-      </c>
-      <c r="O3" t="s">
-        <v>75</v>
-      </c>
-      <c r="P3" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="I3" s="2">
+        <v>0.56589999999999996</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.69950000000000001</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0.68610000000000004</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0.77210000000000001</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0.76049999999999995</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:17">
-      <c r="A4" t="s">
+    <row r="4" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <v>0.502</v>
       </c>
-      <c r="J4">
-        <v>0.6418</v>
-      </c>
-      <c r="K4">
+      <c r="J4" s="2">
+        <v>0.64180000000000004</v>
+      </c>
+      <c r="K4" s="2">
         <v>0.6079</v>
       </c>
-      <c r="L4">
-        <v>0.6278</v>
-      </c>
-      <c r="M4">
-        <v>0.7219</v>
-      </c>
-      <c r="N4">
-        <v>0.7015</v>
-      </c>
-      <c r="O4" t="s">
-        <v>75</v>
-      </c>
-      <c r="P4" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="L4" s="2">
+        <v>0.62780000000000002</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.72189999999999999</v>
+      </c>
+      <c r="N4" s="2">
+        <v>0.70150000000000001</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:17">
-      <c r="A5" t="s">
+    <row r="5" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F5" t="s">
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I5">
-        <v>0.6505</v>
-      </c>
-      <c r="J5">
-        <v>0.7848000000000001</v>
-      </c>
-      <c r="K5">
-        <v>0.7509</v>
-      </c>
-      <c r="L5">
-        <v>0.7714</v>
-      </c>
-      <c r="M5">
-        <v>0.8489</v>
-      </c>
-      <c r="N5">
-        <v>0.855</v>
-      </c>
-      <c r="O5" t="s">
-        <v>75</v>
-      </c>
-      <c r="P5" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="I5" s="2">
+        <v>0.65049999999999997</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.78480000000000005</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.75090000000000001</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.77139999999999997</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.84889999999999999</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q5" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:17">
-      <c r="A6" t="s">
+    <row r="6" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I6">
-        <v>0.4891</v>
-      </c>
-      <c r="J6">
-        <v>0.6347</v>
-      </c>
-      <c r="K6">
-        <v>0.5961</v>
-      </c>
-      <c r="L6">
-        <v>0.6201</v>
-      </c>
-      <c r="M6">
-        <v>0.6853</v>
-      </c>
-      <c r="N6">
-        <v>0.7296</v>
-      </c>
-      <c r="O6" t="s">
-        <v>75</v>
-      </c>
-      <c r="P6" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="I6" s="2">
+        <v>0.48909999999999998</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.63470000000000004</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.59609999999999996</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.62009999999999998</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.68530000000000002</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0.72960000000000003</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q6" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:17">
-      <c r="A7" t="s">
+    <row r="7" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" s="2"/>
+      <c r="F7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="2">
         <v>0.2152</v>
       </c>
-      <c r="J7">
-        <v>0.1433</v>
-      </c>
-      <c r="K7">
-        <v>0.1581</v>
-      </c>
-      <c r="L7">
-        <v>0.1505</v>
-      </c>
-      <c r="M7">
-        <v>0.0757</v>
-      </c>
-      <c r="N7">
-        <v>0.139</v>
-      </c>
-      <c r="O7" t="s">
-        <v>75</v>
-      </c>
-      <c r="P7" t="s">
+      <c r="J7" s="2">
+        <v>0.14330000000000001</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.15809999999999999</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.15049999999999999</v>
+      </c>
+      <c r="M7" s="2">
+        <v>7.5700000000000003E-2</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P7" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="Q7" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="R7" s="2"/>
     </row>
-    <row r="8" spans="1:17">
-      <c r="A8" t="s">
+    <row r="8" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I8">
-        <v>0.539</v>
-      </c>
-      <c r="J8">
+      <c r="I8" s="2">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="J8" s="2">
         <v>0.4451</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="2">
         <v>0.4955</v>
       </c>
-      <c r="L8">
-        <v>0.4545</v>
-      </c>
-      <c r="M8">
+      <c r="L8" s="2">
+        <v>0.45450000000000002</v>
+      </c>
+      <c r="M8" s="2">
         <v>0.6673</v>
       </c>
-      <c r="N8">
-        <v>0.1291</v>
-      </c>
-      <c r="O8" t="s">
-        <v>75</v>
-      </c>
-      <c r="P8" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q8" t="s">
+      <c r="N8" s="2">
+        <v>0.12909999999999999</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q8" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="1:17">
-      <c r="A9" t="s">
+    <row r="9" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I9">
-        <v>0.7111</v>
-      </c>
-      <c r="J9">
-        <v>0.6153999999999999</v>
-      </c>
-      <c r="K9">
-        <v>0.6599</v>
-      </c>
-      <c r="L9">
+      <c r="I9" s="2">
+        <v>0.71109999999999995</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.61539999999999995</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.65990000000000004</v>
+      </c>
+      <c r="L9" s="2">
         <v>0.625</v>
       </c>
-      <c r="M9">
-        <v>0.7735</v>
-      </c>
-      <c r="N9">
-        <v>0.3617</v>
-      </c>
-      <c r="O9" t="s">
-        <v>75</v>
-      </c>
-      <c r="P9" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q9" t="s">
+      <c r="M9" s="2">
+        <v>0.77349999999999997</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0.36170000000000002</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q9" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="R9" s="2"/>
     </row>
-    <row r="10" spans="1:17">
-      <c r="A10" t="s">
+    <row r="10" spans="1:18" ht="48" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F10" t="s">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I10">
-        <v>0.2153</v>
-      </c>
-      <c r="J10">
-        <v>0.1433</v>
-      </c>
-      <c r="K10">
-        <v>0.1581</v>
-      </c>
-      <c r="L10">
-        <v>0.1505</v>
-      </c>
-      <c r="M10">
-        <v>0.0757</v>
-      </c>
-      <c r="N10">
-        <v>0.1388</v>
-      </c>
-      <c r="O10" t="s">
-        <v>75</v>
-      </c>
-      <c r="P10" t="s">
+      <c r="I10" s="2">
+        <v>0.21529999999999999</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.14330000000000001</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.15809999999999999</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0.15049999999999999</v>
+      </c>
+      <c r="M10" s="2">
+        <v>7.5700000000000003E-2</v>
+      </c>
+      <c r="N10" s="2">
+        <v>0.13880000000000001</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P10" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="Q10" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:17">
-      <c r="A11" t="s">
+    <row r="11" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F11" t="s">
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I11">
-        <v>0.2078</v>
-      </c>
-      <c r="J11">
+      <c r="I11" s="2">
+        <v>0.20780000000000001</v>
+      </c>
+      <c r="J11" s="2">
         <v>0.151</v>
       </c>
-      <c r="K11">
-        <v>0.1611</v>
-      </c>
-      <c r="L11">
-        <v>0.1567</v>
-      </c>
-      <c r="M11">
-        <v>0.08119999999999999</v>
-      </c>
-      <c r="N11">
-        <v>0.164</v>
-      </c>
-      <c r="O11" t="s">
-        <v>75</v>
-      </c>
-      <c r="P11" t="s">
+      <c r="K11" s="2">
+        <v>0.16109999999999999</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.15670000000000001</v>
+      </c>
+      <c r="M11" s="2">
+        <v>8.1199999999999994E-2</v>
+      </c>
+      <c r="N11" s="2">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P11" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="Q11" s="2" t="s">
         <v>78</v>
       </c>
+      <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:17">
-      <c r="A12" t="s">
+    <row r="12" spans="1:18" ht="80" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="2">
         <v>0.6573</v>
       </c>
-      <c r="J12">
-        <v>0.7129</v>
-      </c>
-      <c r="K12">
-        <v>0.6972</v>
-      </c>
-      <c r="L12">
-        <v>0.7073</v>
-      </c>
-      <c r="M12">
-        <v>0.7223000000000001</v>
-      </c>
-      <c r="N12">
+      <c r="J12" s="2">
+        <v>0.71289999999999998</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0.69720000000000004</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.70730000000000004</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0.72230000000000005</v>
+      </c>
+      <c r="N12" s="2">
         <v>0.7591</v>
       </c>
-      <c r="O12" t="s">
-        <v>75</v>
-      </c>
-      <c r="P12" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q12" t="s">
+      <c r="O12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q12" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:17">
-      <c r="A13" t="s">
+    <row r="13" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I13">
-        <v>0.6743</v>
-      </c>
-      <c r="J13">
-        <v>0.6989</v>
-      </c>
-      <c r="K13">
-        <v>0.6954</v>
-      </c>
-      <c r="L13">
-        <v>0.6964</v>
-      </c>
-      <c r="M13">
-        <v>0.7377</v>
-      </c>
-      <c r="N13">
-        <v>0.6846</v>
-      </c>
-      <c r="O13" t="s">
-        <v>75</v>
-      </c>
-      <c r="P13" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q13" t="s">
+      <c r="I13" s="2">
+        <v>0.67430000000000001</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.69889999999999997</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.69540000000000002</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.69640000000000002</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.73770000000000002</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0.68459999999999999</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q13" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:17">
-      <c r="A14" t="s">
+    <row r="14" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="2">
         <v>0.7722</v>
       </c>
-      <c r="J14">
-        <v>0.8068</v>
-      </c>
-      <c r="K14">
-        <v>0.7957</v>
-      </c>
-      <c r="L14">
-        <v>0.8033</v>
-      </c>
-      <c r="M14">
-        <v>0.7993</v>
-      </c>
-      <c r="N14">
+      <c r="J14" s="2">
+        <v>0.80679999999999996</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.79569999999999996</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.80330000000000001</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.79930000000000001</v>
+      </c>
+      <c r="N14" s="2">
         <v>0.8488</v>
       </c>
-      <c r="O14" t="s">
-        <v>75</v>
-      </c>
-      <c r="P14" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q14" t="s">
+      <c r="O14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q14" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="R14" s="2"/>
     </row>
-    <row r="15" spans="1:17">
-      <c r="A15" t="s">
+    <row r="15" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="I15">
-        <v>0.9693000000000001</v>
-      </c>
-      <c r="J15">
-        <v>0.976</v>
-      </c>
-      <c r="K15">
-        <v>0.974</v>
-      </c>
-      <c r="L15">
-        <v>0.9752999999999999</v>
-      </c>
-      <c r="M15">
-        <v>0.9761</v>
-      </c>
-      <c r="N15">
-        <v>0.9825</v>
-      </c>
-      <c r="O15" t="s">
-        <v>75</v>
-      </c>
-      <c r="P15" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q15" t="s">
+      <c r="I15" s="2">
+        <v>0.96930000000000005</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0.97529999999999994</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0.97609999999999997</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0.98250000000000004</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q15" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="R15" s="2"/>
     </row>
-    <row r="16" spans="1:17">
-      <c r="A16" t="s">
+    <row r="16" spans="1:18" ht="64" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F16" t="s">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I16">
-        <v>0.726</v>
-      </c>
-      <c r="J16">
-        <v>0.773</v>
-      </c>
-      <c r="K16">
-        <v>0.7633</v>
-      </c>
-      <c r="L16">
-        <v>0.7683</v>
-      </c>
-      <c r="M16">
-        <v>0.8164</v>
-      </c>
-      <c r="N16">
-        <v>0.7766999999999999</v>
-      </c>
-      <c r="O16" t="s">
-        <v>75</v>
-      </c>
-      <c r="P16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q16" t="s">
+      <c r="I16" s="2">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.76329999999999998</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0.76829999999999998</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.81640000000000001</v>
+      </c>
+      <c r="N16" s="2">
+        <v>0.77669999999999995</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q16" s="2" t="s">
         <v>77</v>
       </c>
+      <c r="R16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>